<commit_message>
Update app icons and add launcher icon config
Replaced app icons for macOS and Windows platforms and updated related asset files. Added and configured flutter_launcher_icons in pubspec.yaml to automate icon generation for desktop platforms. Also added new Excel files to assets.
</commit_message>
<xml_diff>
--- a/assets/table_save.xlsx
+++ b/assets/table_save.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eagleimac/Documents/GitHub/excel_file/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\excel_analysis\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C986C5-B3A2-E945-9C9C-78F7EE9C31B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD97807-D462-4351-BE77-C9D1314CCD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="مثال على الاخراج" sheetId="2" r:id="rId1"/>
+    <sheet name="البيانات" sheetId="2" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'مثال على الاخراج'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">البيانات!$A$1:$H$1</definedName>
     <definedName name="الشهر">[1]متغيرات!$E$2:$E$13</definedName>
-    <definedName name="الصنف">'مثال على الاخراج'!#REF!</definedName>
+    <definedName name="الصنف">البيانات!#REF!</definedName>
     <definedName name="الفروع">[1]متغيرات!$F$1:$F$5</definedName>
     <definedName name="رقم_الشهر">[1]متغيرات!$D$2:$D$13</definedName>
   </definedNames>
@@ -580,21 +580,23 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="1"/>
     <col min="2" max="2" width="40" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="10" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="4"/>
-    <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="14.5" style="1"/>
+    <col min="5" max="5" width="14.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="4"/>
+    <col min="7" max="7" width="15.42578125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>